<commit_message>
vault backup: 2024-10-28 01:04:20
</commit_message>
<xml_diff>
--- a/2024-2/Evaluación de proyectos/Excels/Estudio_C3.xlsx
+++ b/2024-2/Evaluación de proyectos/Excels/Estudio_C3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IVAN\Desktop\Codes\Apuntes_2024\2024-2\Evaluación de proyectos\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98049183-B0AE-4896-8217-0CD62725C883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0DDE1B-D783-4FC1-ABCF-2A4EC5A114F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BBB691F9-BAFF-4328-B737-ECDE9CF4B958}"/>
   </bookViews>
@@ -16,8 +16,7 @@
     <sheet name="Plantilla" sheetId="4" r:id="rId1"/>
     <sheet name="Ejercicio 1 control 3" sheetId="7" r:id="rId2"/>
     <sheet name="Ejercicio 2 control 3" sheetId="8" r:id="rId3"/>
-    <sheet name="Ejercicio Ayudantia 7" sheetId="5" r:id="rId4"/>
-    <sheet name="Hoja9" sheetId="9" r:id="rId5"/>
+    <sheet name="Ejercicio Ayudantia 7" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="58">
   <si>
     <t>Año</t>
   </si>
@@ -180,9 +179,6 @@
     <t>BOSTON</t>
   </si>
   <si>
-    <t>ServiCombustible</t>
-  </si>
-  <si>
     <t>ESTADO FINANCIERO BANCO ESTADO</t>
   </si>
   <si>
@@ -193,21 +189,6 @@
   </si>
   <si>
     <t>Forestal Arauco</t>
-  </si>
-  <si>
-    <t>Naviera Andina</t>
-  </si>
-  <si>
-    <t>Bank Inter</t>
-  </si>
-  <si>
-    <t>Bank Europe</t>
-  </si>
-  <si>
-    <t>Bank Global</t>
-  </si>
-  <si>
-    <t>Servicombustible</t>
   </si>
   <si>
     <t>IMPUESTO HOLDING</t>
@@ -241,7 +222,7 @@
   <numFmts count="1">
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +239,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -302,7 +291,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -310,28 +299,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -346,24 +317,19 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
@@ -526,99 +492,6 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>372877</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{345683EA-00A5-5876-9A89-7F8DB04BD783}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10058400" y="66675"/>
-          <a:ext cx="4030477" cy="4962525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>296539</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48CC5DD8-49EE-0F7B-59CD-39C3DC581244}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14012539" y="47626"/>
-          <a:ext cx="3913511" cy="1695450"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1031,24 +904,24 @@
   <dimension ref="A2:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1057,16 +930,16 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="str">
+      <c r="E2" s="10" t="str">
         <f>A2</f>
         <v>?</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1076,14 +949,14 @@
       <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10" t="e">
+      <c r="F3" s="1" t="e">
         <f>_xlfn.COVARIANCE.P(B5:B11,C5:C11)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1" t="e">
+      <c r="H3" s="12" t="e">
         <f>F3/F4</f>
         <v>#DIV/0!</v>
       </c>
@@ -1102,113 +975,113 @@
       <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10" t="e">
+      <c r="F4" s="1" t="e">
         <f>_xlfn.VAR.S(C5:C11)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="1">
         <v>2013</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="16" t="s">
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="1">
         <v>2014</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="16" t="s">
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="1">
         <v>2015</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="1">
         <v>2016</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="16" t="s">
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="1">
         <v>2017</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="16" t="s">
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="1">
         <v>2018</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="16" t="s">
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="1">
         <v>2019</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="16" t="s">
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="10"/>
       <c r="F14" s="2" t="s">
         <v>42</v>
       </c>
@@ -1226,25 +1099,25 @@
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="6" t="s">
         <v>34</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="12" t="s">
+      <c r="G15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1252,25 +1125,25 @@
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="6" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="12" t="s">
+      <c r="G16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1278,25 +1151,25 @@
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" s="12" t="s">
+      <c r="G17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1304,36 +1177,36 @@
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="3">
         <f>SUM(B15:B17)</f>
         <v>0</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="3">
         <f>SUM(D15:D17)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="10" t="e">
+      <c r="G18" s="1" t="e">
         <f>AVERAGE(G15:G17)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="6">
         <f>SUM(H15:H17)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="6">
         <f>SUM(I15:I17)</f>
         <v>0</v>
       </c>
@@ -1342,7 +1215,7 @@
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1350,7 +1223,7 @@
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1358,7 +1231,7 @@
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1366,7 +1239,7 @@
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="11" t="e">
+      <c r="B23" s="5" t="e">
         <f>B22-B21</f>
         <v>#VALUE!</v>
       </c>
@@ -1375,13 +1248,12 @@
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="7"/>
+      <c r="B24" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+      <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
@@ -1411,33 +1283,33 @@
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="12" t="e">
+      <c r="B27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="6" t="e">
         <f>B27+C27</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E27" s="10" t="e">
+      <c r="E27" s="1" t="e">
         <f>D27/D30</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F27" s="3" t="e">
+      <c r="F27" s="1" t="e">
         <f>H3/(1+(1-B20)*(B27/C27))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G27" s="10" t="e">
+      <c r="G27" s="1" t="e">
         <f>H3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H27" s="16" t="e">
+      <c r="H27" s="1" t="e">
         <f>B21+G27*B23</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I27" s="14" t="e">
+      <c r="I27" s="8" t="e">
         <f>(B27/D27)*(1-B20)*B24+(C27/D27)*H27</f>
         <v>#VALUE!</v>
       </c>
@@ -1446,32 +1318,32 @@
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="12" t="e">
+      <c r="B28" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="6" t="e">
         <f t="shared" ref="D28:D30" si="0">B28+C28</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E28" s="10" t="e">
+      <c r="E28" s="1" t="e">
         <f>D28/D30</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="16" t="e">
+      <c r="F28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="1" t="e">
         <f>F28*(1+(1-B20)*(B28/C28))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H28" s="16" t="e">
+      <c r="H28" s="1" t="e">
         <f>B21+G28*B23</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I28" s="14" t="e">
+      <c r="I28" s="8" t="e">
         <f>(B28/D28)*(1-B20)*B24+(C28/D28)*H28</f>
         <v>#VALUE!</v>
       </c>
@@ -1480,86 +1352,86 @@
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="6">
         <f>SUM(D15:D16)</f>
         <v>0</v>
       </c>
-      <c r="C29" s="12" t="str">
+      <c r="C29" s="6" t="str">
         <f>D17</f>
         <v>?</v>
       </c>
-      <c r="D29" s="12" t="e">
+      <c r="D29" s="6" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="E29" s="10" t="e">
+      <c r="E29" s="1" t="e">
         <f>D29/D30</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F29" s="3" t="e">
+      <c r="F29" s="1" t="e">
         <f>G18/(1+(1-B20)*(H19/I19))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G29" s="10" t="e">
+      <c r="G29" s="1" t="e">
         <f>F29*(1+(1-B20)*(B29/C29))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H29" s="16" t="e">
+      <c r="H29" s="1" t="e">
         <f>B21+G29*B23</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I29" s="14" t="e">
+      <c r="I29" s="8" t="e">
         <f>(B29/D29)*(1-B20)*B24+(C29/D29)*H29</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="6">
         <f>SUM(B27:B29)</f>
         <v>0</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="6">
         <f>SUM(C27:C29)</f>
         <v>0</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="10" t="e">
+      <c r="E30" s="1" t="e">
         <f>D30/D30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F30" s="3" t="e">
+      <c r="F30" s="1" t="e">
         <f>F27*E27+F28*E28+F29*E29</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G30" s="10" t="e">
+      <c r="G30" s="1" t="e">
         <f>F30*(1+(1-B20)*(B30/C30))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H30" s="16" t="e">
+      <c r="H30" s="1" t="e">
         <f>B21+G30*B23</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I30" s="14" t="e">
+      <c r="I30" s="8" t="e">
         <f>(B30/D30)*(1-B20)*B24+(C30/D30)*H30</f>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="F13:I13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1570,24 +1442,24 @@
   <dimension ref="A2:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1596,15 +1468,15 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="E2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1614,14 +1486,14 @@
       <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="1">
         <f>_xlfn.COVARIANCE.P(B5:B11,C5:C11)</f>
         <v>3.3673469387755089E-4</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="12">
         <f>F3/F4</f>
         <v>0.29963680387409108</v>
       </c>
@@ -1640,113 +1512,113 @@
       <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="1">
         <f>_xlfn.VAR.S(C5:C11)</f>
         <v>1.1238095238095269E-3</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="1">
         <v>2013</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="1">
         <v>0.02</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="1">
         <v>0.09</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="1">
         <v>2014</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="1">
         <v>0.06</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="1">
         <v>0.08</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="1">
         <v>2015</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="1">
         <v>0.12</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="1">
         <v>2016</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="1">
         <v>0.04</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="1">
         <v>0.13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="1">
         <v>2017</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="1">
         <v>0.12</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="1">
         <v>0.15</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="1">
         <v>2018</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="1">
         <v>0.09</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="1">
         <v>2019</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="1">
         <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="F13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="10"/>
       <c r="F14" s="2" t="s">
         <v>42</v>
       </c>
@@ -1764,25 +1636,25 @@
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="6">
         <v>16500</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="6">
         <v>3800</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="1">
         <v>1.2</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="6">
         <v>5300</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="6">
         <v>4000</v>
       </c>
     </row>
@@ -1790,25 +1662,25 @@
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="6">
         <v>300</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="6">
         <v>3900</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="16">
+        <v>51</v>
+      </c>
+      <c r="G16" s="1">
         <v>1.9</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="6">
         <v>7000</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="6">
         <v>3500</v>
       </c>
     </row>
@@ -1816,25 +1688,25 @@
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="6">
         <v>3200</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="6">
         <v>12300</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="16">
+        <v>52</v>
+      </c>
+      <c r="G17" s="1">
         <v>1.7</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="6">
         <v>6000</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="6">
         <v>4000</v>
       </c>
     </row>
@@ -1842,36 +1714,36 @@
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="3">
         <f>SUM(B15:B17)</f>
         <v>20000</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="3">
         <f>SUM(D15:D17)</f>
         <v>20000</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="1">
         <f>AVERAGE(G15:G17)</f>
         <v>1.5999999999999999</v>
       </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="6">
         <f>SUM(H15:H17)</f>
         <v>18300</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="6">
         <f>SUM(I15:I17)</f>
         <v>11500</v>
       </c>
@@ -1880,7 +1752,7 @@
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="5">
         <v>0.25</v>
       </c>
     </row>
@@ -1888,7 +1760,7 @@
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="5">
         <v>0.02</v>
       </c>
     </row>
@@ -1896,15 +1768,16 @@
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="5">
         <v>0.13</v>
       </c>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="5">
         <f>B22-B21</f>
         <v>0.11</v>
       </c>
@@ -1913,13 +1786,12 @@
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="5">
         <v>7.8E-2</v>
       </c>
-      <c r="E24" s="7"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+      <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
@@ -1949,33 +1821,33 @@
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="6">
         <v>3845</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="6">
         <v>17980</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="6">
         <f>B27+C27</f>
         <v>21825</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="1">
         <f>D27/D30</f>
         <v>0.26785714285714285</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="1">
         <f>H3/(1+(1-B20)*(B27/C27))</f>
         <v>0.25822154376160361</v>
       </c>
-      <c r="G27" s="10">
+      <c r="G27" s="1">
         <f>H3</f>
         <v>0.29963680387409108</v>
       </c>
-      <c r="H27" s="14">
+      <c r="H27" s="8">
         <f>B21+G27*B23</f>
         <v>5.2960048426150014E-2</v>
       </c>
-      <c r="I27" s="14">
+      <c r="I27" s="8">
         <f>(B27/D27)*(1-B20)*B24+(C27/D27)*H27</f>
         <v>5.3936044476617512E-2</v>
       </c>
@@ -1984,32 +1856,32 @@
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="6">
         <v>3975</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="6">
         <v>35680</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="6">
         <f t="shared" ref="D28:D30" si="0">B28+C28</f>
         <v>39655</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="1">
         <f>D28/D30</f>
         <v>0.48668384879725085</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="1">
         <v>1.51</v>
       </c>
-      <c r="G28" s="16">
+      <c r="G28" s="1">
         <f>F28*(1+(1-B20)*(B28/C28))</f>
         <v>1.6361683716367714</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H28" s="8">
         <f>B21+G28*B23</f>
         <v>0.19997852088004484</v>
       </c>
-      <c r="I28" s="14">
+      <c r="I28" s="8">
         <f>(B28/D28)*(1-B20)*B24+(C28/D28)*H28</f>
         <v>0.18579677531206656</v>
       </c>
@@ -2018,72 +1890,72 @@
       <c r="A29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="6">
         <f>SUM(D15:D16)</f>
         <v>7700</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="6">
         <f>D17</f>
         <v>12300</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="6">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="1">
         <f>D29/D30</f>
         <v>0.24545900834560627</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="1">
         <f>G18/(1+(1-B20)*(H19/I19))</f>
         <v>0.72943508424182368</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="1">
         <f>F29*(1+(1-B20)*(B29/C29))</f>
         <v>1.0719137518431676</v>
       </c>
-      <c r="H29" s="14">
+      <c r="H29" s="8">
         <f>B21+G29*B23</f>
         <v>0.13791051270274843</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="8">
         <f>(B29/D29)*(1-B20)*B24+(C29/D29)*H29</f>
         <v>0.10733746531219028</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="6">
         <f>SUM(B27:B29)</f>
         <v>15520</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="6">
         <f>SUM(C27:C29)</f>
         <v>65960</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="6">
         <f t="shared" si="0"/>
         <v>81480</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="1">
         <f>D30/D30</f>
         <v>1</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="1">
         <f>F27*E27+F28*E28+F29*E29</f>
         <v>0.98310550905048444</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="1">
         <f>F30*(1+(1-B20)*(B30/C30))</f>
         <v>1.1565947165299817</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="8">
         <f>B21+G30*B23</f>
         <v>0.14722541881829798</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="8">
         <f>(B30/D30)*(1-B20)*B24+(C30/D30)*H30</f>
         <v>0.13032533904338409</v>
       </c>
@@ -2126,15 +1998,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2143,34 +2015,34 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="1">
         <f>_xlfn.COVARIANCE.P(B5:B9,C5:C9)</f>
         <v>1.1399999999999997E-3</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="12">
         <f>F3/F4</f>
         <v>0.5700000000000004</v>
       </c>
@@ -2186,120 +2058,120 @@
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="1">
         <f>_xlfn.VAR.S(C5:C9)</f>
         <v>1.9999999999999983E-3</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="1">
         <v>2013</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="1">
         <v>0.02</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="1">
         <v>0.09</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="1">
         <v>2014</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="1">
         <v>0.04</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="1">
         <v>2015</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="1">
         <v>0.11</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="1">
         <v>2016</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="1">
         <v>0.09</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="1">
         <v>0.18</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="1">
         <v>2017</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="1">
         <v>0.12</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="1">
         <v>0.15</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="4" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="2" t="s">
         <v>42</v>
       </c>
@@ -2317,26 +2189,26 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="6">
         <v>14500</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="6">
         <v>3500</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="1">
         <v>1.3</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="6">
         <v>5300</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="6">
         <v>4000</v>
       </c>
     </row>
@@ -2344,26 +2216,26 @@
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="6">
         <v>300</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="6">
         <v>1500</v>
       </c>
-      <c r="E14" s="9"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="1">
         <v>1.8</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="6">
         <v>7000</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="6">
         <v>3500</v>
       </c>
     </row>
@@ -2371,26 +2243,26 @@
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="6">
         <v>2200</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="6">
         <v>12000</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="1">
         <v>1.7</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="6">
         <v>6000</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="6">
         <v>4000</v>
       </c>
     </row>
@@ -2398,43 +2270,43 @@
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="3">
         <f>SUM(B13:B15)</f>
         <v>17000</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="3">
         <f>SUM(D13:D15)</f>
         <v>17000</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="8" t="s">
+      <c r="E16" s="4"/>
+      <c r="F16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="1">
         <f>AVERAGE(G13:G15)</f>
         <v>1.5999999999999999</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="6">
         <f>SUM(H13:H15)</f>
         <v>18300</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="6">
         <f>SUM(I13:I15)</f>
         <v>11500</v>
       </c>
@@ -2443,73 +2315,73 @@
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="5">
         <v>0.27</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="5">
         <v>0.08</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="5">
         <v>0.16</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="5">
         <f>B20-B19</f>
         <v>0.08</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="5">
         <v>0.08</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="9"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
+      <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
@@ -2539,33 +2411,33 @@
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="6">
         <v>3890</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="6">
         <v>32589</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="6">
         <f>B25+C25</f>
         <v>36479</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="1">
         <f>D25/D28</f>
         <v>0.50873009232142363</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="1">
         <f>H3/(1+(1-B18)*(B25/C25))</f>
         <v>0.52431305692842278</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="1">
         <f>H3</f>
         <v>0.5700000000000004</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="7">
         <f>B19+G25*B21</f>
         <v>0.12560000000000004</v>
       </c>
-      <c r="I25" s="14">
+      <c r="I25" s="8">
         <f>(B25/D25)*(1-B18)*B22+(C25/D25)*H25</f>
         <v>0.11843401409029858</v>
       </c>
@@ -2574,32 +2446,32 @@
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="6">
         <v>2350</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="6">
         <v>15877</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="6">
         <f t="shared" ref="D26:D28" si="0">B26+C26</f>
         <v>18227</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="1">
         <f>D26/D28</f>
         <v>0.25419072323097092</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="1">
         <f>G26/(1+(1-B18)*(B26/C26))</f>
         <v>0.88443711809009518</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G26" s="1">
         <v>0.98</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="7">
         <f>B19+G26*B21</f>
         <v>0.15839999999999999</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="8">
         <f>(B26/D26)*(1-B18)*B22+(C26/D26)*H26</f>
         <v>0.14550703900806494</v>
       </c>
@@ -2608,710 +2480,74 @@
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="6">
         <f>SUM(D13:D14)</f>
         <v>5000</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="6">
         <f>D15</f>
         <v>12000</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="6">
         <f t="shared" si="0"/>
         <v>17000</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="1">
         <f>D27/D28</f>
         <v>0.23707918444760551</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="1">
         <f>G16/(1+(1-B18)*(H17/I17))</f>
         <v>0.7401745846574681</v>
       </c>
-      <c r="G27" s="10">
+      <c r="G27" s="1">
         <f>F27*(1+(1-B18)*(B27/C27))</f>
         <v>0.96531102082411469</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="7">
         <f>B19+G27*B21</f>
         <v>0.15722488166592918</v>
       </c>
-      <c r="I27" s="14">
+      <c r="I27" s="8">
         <f>(B27/D27)*(1-B18)*B22+(C27/D27)*H27</f>
         <v>0.12815873999947944</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="6">
         <f>SUM(B25:B27)</f>
         <v>11240</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="6">
         <f>SUM(C25:C27)</f>
         <v>60466</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="6">
         <f t="shared" si="0"/>
         <v>71706</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="1">
         <f>D28/D28</f>
         <v>1</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="1">
         <f>F25*E25+F26*E26+F27*E27</f>
         <v>0.66702952743559896</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="1">
         <f>F28*(1+(1-B18)*(B28/C28))</f>
         <v>0.75754503496899916</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="7">
         <f>B19+G28*B21</f>
         <v>0.14060360279751993</v>
       </c>
-      <c r="I28" s="14">
+      <c r="I28" s="8">
         <f>(B28/D28)*(1-B18)*B22+(C28/D28)*H28</f>
         <v>0.12771809118839206</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC58E59C-154B-4F57-A025-2B6AB51EF454}">
-  <dimension ref="A1:I30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="10">
-        <f>_xlfn.COVARIANCE.P(B5:B9,C5:C9)</f>
-        <v>1.0800000000000002E-3</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="1">
-        <f>F3/F4</f>
-        <v>0.84375000000000022</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="str">
-        <f>A2</f>
-        <v>Servicombustible</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="10">
-        <f>_xlfn.VAR.S(C5:C9)</f>
-        <v>1.2799999999999999E-3</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>2018</v>
-      </c>
-      <c r="B5" s="16">
-        <v>0.03</v>
-      </c>
-      <c r="C5" s="16">
-        <v>0.08</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>2019</v>
-      </c>
-      <c r="B6" s="16">
-        <v>0.05</v>
-      </c>
-      <c r="C6" s="16">
-        <v>0.12</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B7" s="16">
-        <v>0.08</v>
-      </c>
-      <c r="C7" s="16">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>2021</v>
-      </c>
-      <c r="B8" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="C8" s="16">
-        <v>0.17</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>2022</v>
-      </c>
-      <c r="B9" s="16">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="C9" s="16">
-        <v>0.16</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="12">
-        <v>30500</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="12">
-        <v>16700</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="16">
-        <v>1.6</v>
-      </c>
-      <c r="H13" s="12">
-        <v>6800</v>
-      </c>
-      <c r="I13" s="12">
-        <v>4700</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="12">
-        <v>400</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="12">
-        <v>1900</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="16">
-        <v>1.8</v>
-      </c>
-      <c r="H14" s="12">
-        <v>7300</v>
-      </c>
-      <c r="I14" s="12">
-        <v>4100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="12">
-        <v>2600</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="12">
-        <v>14900</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="H15" s="12">
-        <v>6500</v>
-      </c>
-      <c r="I15" s="12">
-        <v>4600</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="6">
-        <f>SUM(B13:B15)</f>
-        <v>33500</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="6">
-        <f>SUM(D13:D15)</f>
-        <v>33500</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="10">
-        <f>AVERAGE(G13:G15)</f>
-        <v>1.6333333333333335</v>
-      </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="12">
-        <f>SUM(H13:H15)</f>
-        <v>20600</v>
-      </c>
-      <c r="I17" s="12">
-        <f>SUM(I13:I15)</f>
-        <v>13400</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="11">
-        <v>0.24</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="11">
-        <v>0.03</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="11">
-        <f>B20-B19</f>
-        <v>0.09</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="11">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="12">
-        <v>3900</v>
-      </c>
-      <c r="C26" s="12">
-        <v>6100</v>
-      </c>
-      <c r="D26" s="12">
-        <f>B26+C26</f>
-        <v>10000</v>
-      </c>
-      <c r="E26" s="10">
-        <f>D26/D30</f>
-        <v>0.16806722689075632</v>
-      </c>
-      <c r="F26" s="20">
-        <f>H3/(1+(1-B18)*(B26/C26))</f>
-        <v>0.5678370476610769</v>
-      </c>
-      <c r="G26" s="10">
-        <f>H3</f>
-        <v>0.84375000000000022</v>
-      </c>
-      <c r="H26" s="18">
-        <f>B19+G26*B21</f>
-        <v>0.10593750000000002</v>
-      </c>
-      <c r="I26" s="19">
-        <f>(B26/D26)*(1-B18)*B22+(C26/D26)*H26</f>
-        <v>8.2405875000000003E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="12">
-        <v>4200</v>
-      </c>
-      <c r="C27" s="12">
-        <v>5800</v>
-      </c>
-      <c r="D27" s="12">
-        <f t="shared" ref="D27:D30" si="0">B27+C27</f>
-        <v>10000</v>
-      </c>
-      <c r="E27" s="10">
-        <f>D27/D30</f>
-        <v>0.16806722689075632</v>
-      </c>
-      <c r="F27" s="20">
-        <f>G27/(1+(1-B18)*(B27/C27))</f>
-        <v>0.54826512455516008</v>
-      </c>
-      <c r="G27" s="16">
-        <v>0.85</v>
-      </c>
-      <c r="H27" s="18">
-        <f>B19+G27*B21</f>
-        <v>0.1065</v>
-      </c>
-      <c r="I27" s="19">
-        <f>(B27/D27)*(1-B18)*B22+(C27/D27)*H27</f>
-        <v>8.0921999999999994E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="12">
-        <f>D13+D14</f>
-        <v>18600</v>
-      </c>
-      <c r="C28" s="12">
-        <f>D15</f>
-        <v>14900</v>
-      </c>
-      <c r="D28" s="12">
-        <f>B28+C28</f>
-        <v>33500</v>
-      </c>
-      <c r="E28" s="10">
-        <f>D28/D30</f>
-        <v>0.56302521008403361</v>
-      </c>
-      <c r="F28" s="20">
-        <f>G16/(1+(1-B18)*(H17/I17))</f>
-        <v>0.75325807635829678</v>
-      </c>
-      <c r="G28" s="10">
-        <f>F28*(1+(1-B18)*(B28/C28))</f>
-        <v>1.4678927184657384</v>
-      </c>
-      <c r="H28" s="18">
-        <f>B19+G28*B21</f>
-        <v>0.16211034466191646</v>
-      </c>
-      <c r="I28" s="19">
-        <f>(B28/D28)*(1-B18)*B22+(C28/D28)*H28</f>
-        <v>9.7421018969031492E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="12">
-        <v>2500</v>
-      </c>
-      <c r="C29" s="12">
-        <v>3500</v>
-      </c>
-      <c r="D29" s="12">
-        <f>B29+C29</f>
-        <v>6000</v>
-      </c>
-      <c r="E29" s="16">
-        <f>D29/D30</f>
-        <v>0.10084033613445378</v>
-      </c>
-      <c r="F29" s="20">
-        <f>G29/(1+(1-B18)*(B29/C29))</f>
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="G29" s="10">
-        <v>0.81</v>
-      </c>
-      <c r="H29" s="18">
-        <f>B20+G29*B22</f>
-        <v>0.1686</v>
-      </c>
-      <c r="I29" s="19">
-        <f>(B29/D29)*(1-B19)*B24+(C29/D29)*H29</f>
-        <v>9.8350000000000007E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="12">
-        <f>SUM(B26:B29)</f>
-        <v>29200</v>
-      </c>
-      <c r="C30" s="12">
-        <f>SUM(C26:C29)</f>
-        <v>30300</v>
-      </c>
-      <c r="D30" s="12">
-        <f t="shared" si="0"/>
-        <v>59500</v>
-      </c>
-      <c r="E30" s="10">
-        <f>D30/D30</f>
-        <v>1</v>
-      </c>
-      <c r="F30" s="20">
-        <f>F26*E26+F27*E27+F28*E28</f>
-        <v>0.61168348370025738</v>
-      </c>
-      <c r="G30" s="10">
-        <f>F30*(1+(1-B23)*(B30/C30))</f>
-        <v>1.0361070335786142</v>
-      </c>
-      <c r="H30" s="18">
-        <f>B19+G30*B21</f>
-        <v>0.12324963302207527</v>
-      </c>
-      <c r="I30" s="19">
-        <f>(B30/D30)*(1-B18)*B22+(C30/D30)*H30</f>
-        <v>8.5142586228048406E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3330,7 +2566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E535D25-B662-4A55-9EA2-582511DAA01D}">
   <dimension ref="A2:I29"/>
   <sheetViews>
@@ -3340,20 +2576,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>59</v>
+      <c r="A2" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -3361,16 +2597,16 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="str">
+      <c r="E2" s="10" t="str">
         <f>A2</f>
         <v>ServiCombustibles</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3380,14 +2616,14 @@
       <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="1">
         <f>_xlfn.COVARIANCE.P(B5:B9,C5:C9)</f>
         <v>1.0800000000000002E-3</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="12">
         <f>F3/F4</f>
         <v>0.84375000000000022</v>
       </c>
@@ -3406,91 +2642,91 @@
       <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="1">
         <f>_xlfn.VAR.S(C5:C9)</f>
         <v>1.2799999999999999E-3</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="1">
         <v>2018</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="1">
         <v>0.03</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="1">
         <v>0.08</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="1">
         <v>2019</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="1">
         <v>0.05</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="1">
         <v>0.12</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="1">
         <v>2020</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="1">
         <v>0.08</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="1">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="1">
         <v>2021</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="1">
         <v>0.1</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="1">
         <v>0.17</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="1">
         <v>2022</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="1">
         <v>0.16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="F11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="10"/>
       <c r="F12" s="2" t="s">
         <v>42</v>
       </c>
@@ -3508,25 +2744,25 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="6">
         <v>30500</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="6">
         <v>16700</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="16">
+        <v>54</v>
+      </c>
+      <c r="G13" s="1">
         <v>1.6</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="6">
         <v>6800</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="6">
         <v>4700</v>
       </c>
     </row>
@@ -3534,25 +2770,25 @@
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="6">
         <v>400</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="6">
         <v>1900</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="16">
+        <v>55</v>
+      </c>
+      <c r="G14" s="1">
         <v>1.8</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="6">
         <v>7300</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="6">
         <v>4100</v>
       </c>
     </row>
@@ -3560,25 +2796,25 @@
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="6">
         <v>2600</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="6">
         <v>14900</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="16">
+        <v>56</v>
+      </c>
+      <c r="G15" s="1">
         <v>1.5</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="6">
         <v>6500</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="6">
         <v>4600</v>
       </c>
     </row>
@@ -3586,36 +2822,36 @@
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="3">
         <f>SUM(B13:B15)</f>
         <v>33500</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="3">
         <f>SUM(D13:D15)</f>
         <v>33500</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="1">
         <f>AVERAGE(G13:G15)</f>
         <v>1.6333333333333335</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="6">
         <f>SUM(H13:H15)</f>
         <v>20600</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="6">
         <f>SUM(I13:I15)</f>
         <v>13400</v>
       </c>
@@ -3624,13 +2860,13 @@
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="5">
         <v>0.24</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="11">
+        <v>50</v>
+      </c>
+      <c r="D18" s="5">
         <v>0.28000000000000003</v>
       </c>
     </row>
@@ -3638,7 +2874,7 @@
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="5">
         <v>0.04</v>
       </c>
     </row>
@@ -3646,7 +2882,7 @@
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="5">
         <v>0.13</v>
       </c>
     </row>
@@ -3654,7 +2890,7 @@
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="5">
         <f>B20-B19</f>
         <v>0.09</v>
       </c>
@@ -3663,13 +2899,12 @@
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="5">
         <v>0.06</v>
       </c>
-      <c r="E22" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
+      <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
@@ -3697,177 +2932,177 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="12">
+        <v>53</v>
+      </c>
+      <c r="B25" s="6">
         <v>3900</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="6">
         <v>6100</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="6">
         <f>B25+C25</f>
         <v>10000</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="1">
         <f>D25/D29</f>
         <v>0.16806722689075632</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="1">
         <f>H3/(1+(1-B18)*(B25/C25))</f>
         <v>0.5678370476610769</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="1">
         <f>H3</f>
         <v>0.84375000000000022</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="5">
         <f>B19+G25*B21</f>
         <v>0.11593750000000003</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="9">
         <f>(B25/D25)*(1-B18)*B22+(C25/D25)*H25</f>
         <v>8.8505875000000012E-2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="12">
+        <v>49</v>
+      </c>
+      <c r="B26" s="6">
         <v>4200</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="6">
         <v>5800</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="6">
         <f>B26+C26</f>
         <v>10000</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="1">
         <f>D26/D29</f>
         <v>0.16806722689075632</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="1">
         <f>G26/(1+(1-B18)*(B26/C26))</f>
         <v>0.54826512455516008</v>
       </c>
-      <c r="G26" s="10">
+      <c r="G26" s="1">
         <v>0.85</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="5">
         <f>B19+G26*B21</f>
         <v>0.11649999999999999</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="9">
         <f>(B26/D26)*(1-B18)*B22+(C26/D26)*H26</f>
         <v>8.6721999999999994E-2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="12">
+        <v>57</v>
+      </c>
+      <c r="B27" s="6">
         <v>2500</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="6">
         <v>3500</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="6">
         <f t="shared" ref="D27:D29" si="0">B27+C27</f>
         <v>6000</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="1">
         <f>D27/D29</f>
         <v>0.10084033613445378</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="1">
         <f>G27/(1+(1-B18)*(B27/C27))</f>
         <v>0.52500000000000002</v>
       </c>
-      <c r="G27" s="16">
+      <c r="G27" s="1">
         <v>0.81</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="5">
         <f>B19+G27*B21</f>
         <v>0.1129</v>
       </c>
-      <c r="I27" s="15">
+      <c r="I27" s="9">
         <f>(B27/D27)*(1-B18)*B22+(C27/D27)*H27</f>
         <v>8.4858333333333341E-2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="12">
+        <v>48</v>
+      </c>
+      <c r="B28" s="6">
         <f>SUM(D13:D14)</f>
         <v>18600</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="6">
         <f>D15</f>
         <v>14900</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="6">
         <f t="shared" si="0"/>
         <v>33500</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="1">
         <f>D28/D29</f>
         <v>0.56302521008403361</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="1">
         <f>G16/(1+(1-B18)*(H17/I17))</f>
         <v>0.75325807635829678</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="1">
         <f>F28*(1+(1-B18)*(B28/C28))</f>
         <v>1.4678927184657384</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="5">
         <f>B19+G28*B21</f>
         <v>0.17211034466191646</v>
       </c>
-      <c r="I28" s="15">
+      <c r="I28" s="9">
         <f>(B28/D28)*(1-B18)*B22+(C28/D28)*H28</f>
         <v>0.10186878016306135</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="6">
         <f>SUM(B25:B28)</f>
         <v>29200</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="6">
         <f>SUM(C25:C28)</f>
         <v>30300</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="6">
         <f t="shared" si="0"/>
         <v>59500</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="1">
         <f>D29/D29</f>
         <v>1</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="1">
         <f>F25*E25+F27*E27+F28*E28</f>
         <v>0.57247926108594471</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="1">
         <f>F29*(1+(1-D18)*(B29/C29))</f>
         <v>0.96970051471864771</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="5">
         <f>B19+G29*B21</f>
         <v>0.12727304632467829</v>
       </c>
-      <c r="I29" s="15">
+      <c r="I29" s="9">
         <f>(B29/D29)*(1-D18)*B22+(C29/D29)*H29</f>
         <v>8.6013668968701718E-2</v>
       </c>

</xml_diff>